<commit_message>
Change schottky diode on fixed,10V,24mA,275nm design.
</commit_message>
<xml_diff>
--- a/fixed/10V_regulator/275nm_SU_CULBN2_24mA/production/ver_0p1_rev_2/BOM_JLCPCB_275nm_SU_CULBN2_24mA.xlsx
+++ b/fixed/10V_regulator/275nm_SU_CULBN2_24mA/production/ver_0p1_rev_2/BOM_JLCPCB_275nm_SU_CULBN2_24mA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -119,7 +119,10 @@
     <t xml:space="preserve">D2</t>
   </si>
   <si>
-    <t xml:space="preserve">C2837790</t>
+    <t xml:space="preserve">SOD-523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C345957</t>
   </si>
   <si>
     <t xml:space="preserve">4-Pin Connector, JST SM04B-SRSS-TB</t>
@@ -131,7 +134,7 @@
     <t xml:space="preserve">SMD,P=1mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C160404</t>
+    <t xml:space="preserve">C145956</t>
   </si>
   <si>
     <t xml:space="preserve">22uH Inductor</t>
@@ -461,7 +464,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="6:6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -550,10 +553,10 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>1</v>
@@ -561,16 +564,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>2</v>
@@ -578,16 +581,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1</v>
@@ -595,16 +598,16 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>1</v>
@@ -612,16 +615,16 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>1</v>
@@ -629,16 +632,16 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>1</v>
@@ -646,16 +649,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>1</v>
@@ -663,16 +666,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>2</v>
@@ -680,16 +683,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
@@ -697,16 +700,16 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>1</v>
@@ -714,16 +717,16 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>1</v>

</xml_diff>